<commit_message>
Start calibrating distance sensors. Need to redo with moving average
</commit_message>
<xml_diff>
--- a/Code/Calibration/DistanceSensorCalibration.xlsx
+++ b/Code/Calibration/DistanceSensorCalibration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kinblandford/Documents/Arduino/mechatronics-goats/Code/Calibration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33BECDA6-7DC2-2E4F-BB2F-A074F6F18FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C344126-62D2-804E-9307-A9558165CEC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17260" xr2:uid="{A9049DBD-7243-9D4D-A141-C415C5CAD369}"/>
+    <workbookView xWindow="13660" yWindow="980" windowWidth="13460" windowHeight="17260" xr2:uid="{A9049DBD-7243-9D4D-A141-C415C5CAD369}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,26 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Inches</t>
+  </si>
+  <si>
+    <t>LeftReading</t>
+  </si>
+  <si>
+    <t>RightReading</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Interference Min Distance</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -66,8 +86,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,12 +423,503 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C1BFEC-3E60-AD43-9FB6-810D5B0BB7A3}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="B2" s="1">
+        <v>420</v>
+      </c>
+      <c r="C2" s="1">
+        <v>460</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="B3" s="1">
+        <v>388</v>
+      </c>
+      <c r="C3" s="1">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="B4" s="1">
+        <v>340</v>
+      </c>
+      <c r="C4" s="1">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>308</v>
+      </c>
+      <c r="C5" s="1">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>1.125</v>
+      </c>
+      <c r="B6" s="1">
+        <v>278</v>
+      </c>
+      <c r="C6" s="1">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="B7" s="1">
+        <v>260</v>
+      </c>
+      <c r="C7" s="1">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>1.375</v>
+      </c>
+      <c r="B8" s="1">
+        <v>243</v>
+      </c>
+      <c r="C8" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="B9" s="1">
+        <v>224</v>
+      </c>
+      <c r="C9" s="1">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>1.625</v>
+      </c>
+      <c r="B10" s="1">
+        <v>188</v>
+      </c>
+      <c r="C10" s="1">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="B11" s="1">
+        <v>177</v>
+      </c>
+      <c r="C11" s="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>160</v>
+      </c>
+      <c r="C13" s="1">
+        <v>204</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>2.125</v>
+      </c>
+      <c r="B14" s="1">
+        <v>153</v>
+      </c>
+      <c r="C14" s="1">
+        <v>194</v>
+      </c>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>2.25</v>
+      </c>
+      <c r="B15" s="1">
+        <v>148</v>
+      </c>
+      <c r="C15" s="1">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>2.375</v>
+      </c>
+      <c r="B16" s="1">
+        <v>144</v>
+      </c>
+      <c r="C16" s="1">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>140</v>
+      </c>
+      <c r="C17" s="1">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>2.625</v>
+      </c>
+      <c r="B18" s="1">
+        <v>130</v>
+      </c>
+      <c r="C18" s="1">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>2.75</v>
+      </c>
+      <c r="B19" s="1">
+        <v>111</v>
+      </c>
+      <c r="C19" s="1">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>2.875</v>
+      </c>
+      <c r="B20" s="1">
+        <v>120</v>
+      </c>
+      <c r="C20" s="1">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <f>A20+1/8</f>
+        <v>3</v>
+      </c>
+      <c r="B21" s="1">
+        <v>115</v>
+      </c>
+      <c r="C21" s="1">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <f t="shared" ref="A22:A47" si="0">A21+1/8</f>
+        <v>3.125</v>
+      </c>
+      <c r="B22" s="1">
+        <v>116</v>
+      </c>
+      <c r="C22" s="1">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <f t="shared" si="0"/>
+        <v>3.25</v>
+      </c>
+      <c r="B23" s="1">
+        <v>114</v>
+      </c>
+      <c r="C23" s="1">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <f t="shared" si="0"/>
+        <v>3.375</v>
+      </c>
+      <c r="B24" s="1">
+        <v>108</v>
+      </c>
+      <c r="C24" s="1">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="B25" s="1">
+        <v>109</v>
+      </c>
+      <c r="C25" s="1">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <f t="shared" si="0"/>
+        <v>3.625</v>
+      </c>
+      <c r="B26" s="1">
+        <v>104</v>
+      </c>
+      <c r="C26" s="1">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <f t="shared" si="0"/>
+        <v>3.75</v>
+      </c>
+      <c r="B27" s="1">
+        <v>103</v>
+      </c>
+      <c r="C27" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <f t="shared" si="0"/>
+        <v>3.875</v>
+      </c>
+      <c r="B28" s="1">
+        <v>102</v>
+      </c>
+      <c r="C28" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B29" s="1">
+        <v>98</v>
+      </c>
+      <c r="C29" s="1">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <f t="shared" si="0"/>
+        <v>4.125</v>
+      </c>
+      <c r="B30" s="1">
+        <v>95</v>
+      </c>
+      <c r="C30" s="1">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <f t="shared" si="0"/>
+        <v>4.25</v>
+      </c>
+      <c r="B31" s="1">
+        <v>87</v>
+      </c>
+      <c r="C31" s="1">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <f t="shared" si="0"/>
+        <v>4.375</v>
+      </c>
+      <c r="B32" s="1">
+        <v>94</v>
+      </c>
+      <c r="C32" s="1">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="B33" s="1">
+        <v>92</v>
+      </c>
+      <c r="C33" s="1">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <f t="shared" si="0"/>
+        <v>4.625</v>
+      </c>
+      <c r="B34" s="1">
+        <v>87</v>
+      </c>
+      <c r="C34" s="1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <f t="shared" si="0"/>
+        <v>4.75</v>
+      </c>
+      <c r="B35" s="1">
+        <v>86</v>
+      </c>
+      <c r="C35" s="1">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <f t="shared" si="0"/>
+        <v>4.875</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B37" s="1">
+        <v>88</v>
+      </c>
+      <c r="C37" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <f t="shared" si="0"/>
+        <v>5.125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <f t="shared" si="0"/>
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <f t="shared" si="0"/>
+        <v>5.375</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <f t="shared" si="0"/>
+        <v>5.5</v>
+      </c>
+      <c r="B41">
+        <v>80</v>
+      </c>
+      <c r="C41">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <f t="shared" si="0"/>
+        <v>5.625</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <f t="shared" si="0"/>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <f t="shared" si="0"/>
+        <v>5.875</v>
+      </c>
+      <c r="B44">
+        <v>70</v>
+      </c>
+      <c r="C44">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>